<commit_message>
fixed (entry error) enter_user does now take secific user by index
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="A2:H6"/>
@@ -482,6 +482,36 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>veronica</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>soloduha</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>veronica</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>soloduha</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Tue Apr 19 22:14:07 2022</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>